<commit_message>
Cleaning for the pypi package
</commit_message>
<xml_diff>
--- a/build/lib/simgen/params/QC-age-sexe.xlsx
+++ b/build/lib/simgen/params/QC-age-sexe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Tapageur/Dropbox (CEDIA)/OLG_CAN/demo/raw/isq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmichaud/Dropbox (CEDIA)/OLG_CAN/demo/simgen/simgen/params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B40CCE4-76DB-E84C-98D0-4C1FEC518910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C808141-9D7B-C248-985C-C3F84D518947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="1000" windowWidth="29000" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9720" yWindow="460" windowWidth="29000" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">age!$A$5:$C$152</definedName>
     <definedName name="ExternalData_1" localSheetId="0">age!$A$6:$DC$152</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -633,13 +641,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:DD161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1423,7 +1432,7 @@
       </c>
       <c r="DC5" s="23"/>
     </row>
-    <row r="6" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1971</v>
       </c>
@@ -1746,7 +1755,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="7" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1971</v>
       </c>
@@ -2392,7 +2401,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="9" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>1972</v>
       </c>
@@ -2715,7 +2724,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="10" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>1972</v>
       </c>
@@ -3361,7 +3370,7 @@
         <v>30.3</v>
       </c>
     </row>
-    <row r="12" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>1973</v>
       </c>
@@ -3684,7 +3693,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="13" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>1973</v>
       </c>
@@ -4330,7 +4339,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="15" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>1974</v>
       </c>
@@ -4653,7 +4662,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="16" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>1974</v>
       </c>
@@ -5299,7 +5308,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="18" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>1975</v>
       </c>
@@ -5622,7 +5631,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="19" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>1975</v>
       </c>
@@ -6268,7 +6277,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="21" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>1976</v>
       </c>
@@ -6591,7 +6600,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="22" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>1976</v>
       </c>
@@ -7237,7 +7246,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="24" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>1977</v>
       </c>
@@ -7560,7 +7569,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="25" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>1977</v>
       </c>
@@ -8206,7 +8215,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="27" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>1978</v>
       </c>
@@ -8529,7 +8538,7 @@
         <v>31.1</v>
       </c>
     </row>
-    <row r="28" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>1978</v>
       </c>
@@ -9175,7 +9184,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>1979</v>
       </c>
@@ -9498,7 +9507,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="31" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>1979</v>
       </c>
@@ -10144,7 +10153,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>1980</v>
       </c>
@@ -10467,7 +10476,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="34" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>1980</v>
       </c>
@@ -11113,7 +11122,7 @@
         <v>32.6</v>
       </c>
     </row>
-    <row r="36" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>1981</v>
       </c>
@@ -11436,7 +11445,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="37" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>1981</v>
       </c>
@@ -12082,7 +12091,7 @@
         <v>32.9</v>
       </c>
     </row>
-    <row r="39" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>1982</v>
       </c>
@@ -12405,7 +12414,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="40" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>1982</v>
       </c>
@@ -13051,7 +13060,7 @@
         <v>33.200000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>1983</v>
       </c>
@@ -13374,7 +13383,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="43" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>1983</v>
       </c>
@@ -14020,7 +14029,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="45" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>1984</v>
       </c>
@@ -14343,7 +14352,7 @@
         <v>32.700000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>1984</v>
       </c>
@@ -14989,7 +14998,7 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>1985</v>
       </c>
@@ -15312,7 +15321,7 @@
         <v>32.9</v>
       </c>
     </row>
-    <row r="49" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>1985</v>
       </c>
@@ -15958,7 +15967,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="51" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>1986</v>
       </c>
@@ -16281,7 +16290,7 @@
         <v>33.200000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>1986</v>
       </c>
@@ -16927,7 +16936,7 @@
         <v>34.4</v>
       </c>
     </row>
-    <row r="54" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>1987</v>
       </c>
@@ -17250,7 +17259,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="55" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>1987</v>
       </c>
@@ -17896,7 +17905,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="57" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>1988</v>
       </c>
@@ -18219,7 +18228,7 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>1988</v>
       </c>
@@ -18865,7 +18874,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>1989</v>
       </c>
@@ -19188,7 +19197,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="61" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>1989</v>
       </c>
@@ -19834,7 +19843,7 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>1990</v>
       </c>
@@ -20157,7 +20166,7 @@
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>1990</v>
       </c>
@@ -20803,7 +20812,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="66" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>1991</v>
       </c>
@@ -21126,7 +21135,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="67" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>1991</v>
       </c>
@@ -21772,7 +21781,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="69" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>1992</v>
       </c>
@@ -22095,7 +22104,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="70" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>1992</v>
       </c>
@@ -22741,7 +22750,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="72" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>1993</v>
       </c>
@@ -23064,7 +23073,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="73" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>1993</v>
       </c>
@@ -23710,7 +23719,7 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="75" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>1994</v>
       </c>
@@ -24033,7 +24042,7 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="76" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>1994</v>
       </c>
@@ -24679,7 +24688,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="78" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>1995</v>
       </c>
@@ -25002,7 +25011,7 @@
         <v>35.4</v>
       </c>
     </row>
-    <row r="79" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>1995</v>
       </c>
@@ -25648,7 +25657,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="81" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>1996</v>
       </c>
@@ -25971,7 +25980,7 @@
         <v>35.6</v>
       </c>
     </row>
-    <row r="82" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>1996</v>
       </c>
@@ -26617,7 +26626,7 @@
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>1997</v>
       </c>
@@ -26940,7 +26949,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="85" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>1997</v>
       </c>
@@ -27586,7 +27595,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="87" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>1998</v>
       </c>
@@ -27909,7 +27918,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="88" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>1998</v>
       </c>
@@ -28555,7 +28564,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="90" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>1999</v>
       </c>
@@ -28878,7 +28887,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="91" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>1999</v>
       </c>
@@ -29524,7 +29533,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>2000</v>
       </c>
@@ -29847,7 +29856,7 @@
         <v>36.9</v>
       </c>
     </row>
-    <row r="94" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>2000</v>
       </c>
@@ -30493,7 +30502,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="96" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>2001</v>
       </c>
@@ -30816,7 +30825,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>2001</v>
       </c>
@@ -31462,7 +31471,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="99" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>2002</v>
       </c>
@@ -31785,7 +31794,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="100" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>2002</v>
       </c>
@@ -32431,7 +32440,7 @@
         <v>38.700000000000003</v>
       </c>
     </row>
-    <row r="102" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>2003</v>
       </c>
@@ -32754,7 +32763,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="103" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>2003</v>
       </c>
@@ -33400,7 +33409,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>2004</v>
       </c>
@@ -33723,7 +33732,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="106" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>2004</v>
       </c>
@@ -34369,7 +34378,7 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="108" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>2005</v>
       </c>
@@ -34692,7 +34701,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="109" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>2005</v>
       </c>
@@ -35338,7 +35347,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="111" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>2006</v>
       </c>
@@ -35661,7 +35670,7 @@
         <v>38.700000000000003</v>
       </c>
     </row>
-    <row r="112" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>2006</v>
       </c>
@@ -36307,7 +36316,7 @@
         <v>39.799999999999997</v>
       </c>
     </row>
-    <row r="114" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>2007</v>
       </c>
@@ -36630,7 +36639,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="115" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>2007</v>
       </c>
@@ -37276,7 +37285,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="117" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>2008</v>
       </c>
@@ -37599,7 +37608,7 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="118" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>2008</v>
       </c>
@@ -38245,7 +38254,7 @@
         <v>40.299999999999997</v>
       </c>
     </row>
-    <row r="120" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>2009</v>
       </c>
@@ -38568,7 +38577,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="121" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>2009</v>
       </c>
@@ -39214,7 +39223,7 @@
         <v>40.5</v>
       </c>
     </row>
-    <row r="123" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>2010</v>
       </c>
@@ -39537,7 +39546,7 @@
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="124" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>2010</v>
       </c>
@@ -40183,7 +40192,7 @@
         <v>40.700000000000003</v>
       </c>
     </row>
-    <row r="126" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>2011</v>
       </c>
@@ -40506,7 +40515,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="127" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>2011</v>
       </c>
@@ -41152,7 +41161,7 @@
         <v>40.9</v>
       </c>
     </row>
-    <row r="129" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>2012</v>
       </c>
@@ -41475,7 +41484,7 @@
         <v>40.1</v>
       </c>
     </row>
-    <row r="130" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>2012</v>
       </c>
@@ -42121,7 +42130,7 @@
         <v>41.1</v>
       </c>
     </row>
-    <row r="132" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>2013</v>
       </c>
@@ -42444,7 +42453,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="133" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>2013</v>
       </c>
@@ -43090,7 +43099,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="135" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>2014</v>
       </c>
@@ -43413,7 +43422,7 @@
         <v>40.6</v>
       </c>
     </row>
-    <row r="136" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>2014</v>
       </c>
@@ -44059,7 +44068,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="138" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>2015</v>
       </c>
@@ -44382,7 +44391,7 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="139" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>2015</v>
       </c>
@@ -45028,7 +45037,7 @@
         <v>41.7</v>
       </c>
     </row>
-    <row r="141" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>2016</v>
       </c>
@@ -45351,7 +45360,7 @@
         <v>41.1</v>
       </c>
     </row>
-    <row r="142" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>2016</v>
       </c>
@@ -45997,7 +46006,7 @@
         <v>41.9</v>
       </c>
     </row>
-    <row r="144" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:107" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>2017</v>
       </c>
@@ -46320,7 +46329,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="145" spans="1:108" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:108" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>2017</v>
       </c>
@@ -46966,7 +46975,7 @@
         <v>42.1</v>
       </c>
     </row>
-    <row r="147" spans="1:108" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:108" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>2018</v>
       </c>
@@ -47289,7 +47298,7 @@
         <v>41.4</v>
       </c>
     </row>
-    <row r="148" spans="1:108" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:108" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>2018</v>
       </c>
@@ -47935,7 +47944,7 @@
         <v>42.3</v>
       </c>
     </row>
-    <row r="150" spans="1:108" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:108" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>2019</v>
       </c>
@@ -48258,7 +48267,7 @@
         <v>41.6</v>
       </c>
     </row>
-    <row r="151" spans="1:108" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:108" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>2019</v>
       </c>
@@ -49149,7 +49158,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:C152" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A5:C152" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:DC147">
     <sortCondition ref="A4:A147"/>
     <sortCondition ref="C4:C147"/>

</xml_diff>